<commit_message>
Completed final 2 scrapes, initial 7/7 complete
</commit_message>
<xml_diff>
--- a/mi/utils/Kubrick MI Data.xlsx
+++ b/mi/utils/Kubrick MI Data.xlsx
@@ -11,6 +11,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="scrape_bettergov" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="scrape_capco" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="infosys" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="kubrick" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="iqvia" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cambridge_consultants" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -7354,4 +7357,1129 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>practices</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>services</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Data Product Management</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Business Analysis &amp; Business Process Mining</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Data Product Management</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Requirements Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Data Product Management</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Agile Product Management</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Data Product Management</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Change &amp; Risk Management</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Data Product Management</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Data Product Testing &amp; Validation</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Data Product Management</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Data Product Launch &amp; Deployment</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Data Product Management</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Data Product Lifecycle Management</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Data Engineering</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Modern Data Architecture &amp; Data Modelling</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Data Engineering</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Data Connectivity and Integration</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Data Engineering</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Cloud Data Warehouse and Lake Development</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Data Engineering</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DataOps</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Data Engineering</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Data Orchestration</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Data Engineering</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Data Streaming​</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Data Engineering</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Scalability &amp; Performance Optimisation</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Data Engineering</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Database Design &amp; Development​</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Data &amp; AI Governance</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Data Governance Frameworks &amp; Policy</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Data &amp; AI Governance</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Policy-as-Code</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Data &amp; AI Governance</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Master Data &amp; Reference Data Management</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Data &amp; AI Governance</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Data Quality Management</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Data &amp; AI Governance</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Data Cataloging &amp; Lineage</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Data &amp; AI Governance</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Data Privacy &amp; Compliance</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Data &amp; AI Governance</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Data Domain Modelling</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Advanced Analytics</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Data Analysis &amp; Insights​</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Advanced Analytics</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Advanced Data Visualisation</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Advanced Analytics</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Decision Intelligence​</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Advanced Analytics</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Knowledge Graph Development​</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Advanced Analytics</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Digital Twins​</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Advanced Analytics</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Data Storytelling​</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Advanced Analytics</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Self-service Enablement</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>GenAI &amp; MLOps</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Feature Engineering​</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>GenAI &amp; MLOps</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Model Development​</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>GenAI &amp; MLOps</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ML Engineering ​</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>GenAI &amp; MLOps</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>LLMOps​</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>GenAI &amp; MLOps</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>LLM Integration &amp; Fine Tuning​</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>GenAI &amp; MLOps</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Prompt Engineering​</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>GenAI &amp; MLOps</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>AI Ethics &amp; Compliance</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Cloud</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Cloud Design &amp; Deployment​</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Cloud</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Cloud Migration​</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Cloud</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Cloud Infra Optimization​</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Cloud</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>CI/CD​</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Cloud</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>FinOps &amp; Sustainability​</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Cloud</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Cloud Security &amp; Compliance​</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Cloud</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>SRE</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>practices</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>services</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Clinical Research</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Monitoring</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Clinical Research</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ClinicalOperations</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Clinical Research</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Clinical Project Management &amp; Leadership</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Clinical Research</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Clinical DataManagement</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Clinical Research</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>StatisticalServices</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Technology &amp; Analytics</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>InformationSecurity</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Technology &amp; Analytics</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>DevOps</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Technology &amp; Analytics</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Software Development Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Technology &amp; Analytics</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Software QA and Test Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Technology &amp; Analytics</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>AI and Machine Learning</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Consulting</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Commercial Consulting</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Consulting</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Real World Consulting</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Consulting</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Technical Consulting</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>practices</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>services</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>5G and wireless connectivity</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Radio systems</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>5G and wireless connectivity</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Connectivity and IOT</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>5G and wireless connectivity</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Digital signal processing</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>5G and wireless connectivity</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AI and analytics</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5G and wireless connectivity</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Strategic advice</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Advanced computing</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ASICs and electronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Advanced computing</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Optics and photonics</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Advanced computing</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Physical sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Advanced computing</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>AI and analytics</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>AI and data analytics</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>AI and analytics</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>AI and data analytics</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Simulation</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>AI and data analytics</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Connectivity and IoT</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>AI and data analytics</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Sensing</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>AI and data analytics</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Electronics and ASICs</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Biotechnology</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Cell and gene therapy</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Biotechnology</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Synthetic biology</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Biotechnology</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>AI and analytics</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Biotechnology</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Physical sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Biotechnology</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Simulation</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Biotechnology</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Strategic advice</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Digital transformation</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Digital services</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Digital transformation</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Digital security</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Digital transformation</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>AI and analytics</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Digital transformation</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Extended reality (XR)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Digital transformation</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>User experience (UX)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Digital transformation</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Connectivity and IOT</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Quantum technology</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Optics and photonics</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Quantum technology</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Physical sciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Quantum technology</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Product realisation</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Quantum technology</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Strategic advice</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>